<commit_message>
Added text and images
</commit_message>
<xml_diff>
--- a/coling2016/props/Ebates-COLING-2016-results.xlsx
+++ b/coling2016/props/Ebates-COLING-2016-results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2420" windowWidth="30840" windowHeight="16620" tabRatio="630" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="630"/>
   </bookViews>
   <sheets>
     <sheet name="DatasetStats" sheetId="14" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="74">
   <si>
     <t>Categories</t>
   </si>
@@ -32,24 +32,12 @@
     <t>NB</t>
   </si>
   <si>
-    <t>Logistic with ElasticNet (one vs all)</t>
-  </si>
-  <si>
-    <t>Logistic with L1 (one vs one)</t>
-  </si>
-  <si>
     <t>GBT</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
     <t>WordUnigramCount</t>
   </si>
   <si>
-    <t>CNN</t>
-  </si>
-  <si>
     <t>Ebates data</t>
   </si>
   <si>
@@ -200,243 +188,6 @@
     <t>Women's Clothing &gt; Clothing</t>
   </si>
   <si>
-    <t>Air_Conditioners_30501&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Arts_Crafts_&amp;_Sewing_30401&gt;Home_Decor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Arts_Crafts_&amp;_Sewing_30401&gt;Home_Décor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Bar_&amp;_Wine_accessories_30601&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Bath_Rugs_&amp;_Mats_30202&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Bathroom_Accessories_30201&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Bedroom_&amp;_Mattresses_30203&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Bedroom_30301&gt;Furniture_30300&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Blankets_&amp;_Throws_30204&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Building_Supplies_30513&gt;Tools_30510&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Coffee_Makers_30102&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Cooking_Utensils_&amp;_Tools_30603&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Cookware_&amp;_Bakeware_30604&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Cutlery_&amp;_Knives_30605&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Deep_Fryers_30104&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Dishwashers_30115&gt;Large_Appliances_30114&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Drinkware_&amp;_Glassware_30607&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Décor_30704&gt;Patio_&amp;_Garden_30700&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Fine_Art_30402&gt;Home_Décor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Flatware_&amp;_Silverware_30608&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Food_Processors_30105&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Food_Storage_30609&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Freezers_&amp;_Ice_Makers_30116&gt;Large_Appliances_30114&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Furniture_30703&gt;Patio_&amp;_Garden_30700&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Game_Room_&amp;_Bar_30302&gt;Furniture_30300&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Gardening_&amp;_Lawn_Care_30701&gt;Patio_&amp;_Garden_30700&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Griddles_&amp;_Grills_30106&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Grill_&amp;_Outdoors_Cooking_30702&gt;Patio_&amp;_Garden_30700&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Hand_Tools_30514&gt;Tools_30510&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Hardware_30504&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Heating_Cooling_&amp;_Air_Quality_30505&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Home_Décor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Home_Office_30303&gt;Furniture_30300&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Juicers_&amp;_Blenders_30107&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Kids'_Room_30304&gt;Furniture_30300&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Kitchen_&amp;_Dining_30305&gt;Furniture_30300&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Kitchen_Gadgets_30606&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Lamps_&amp;_Light_Fixtures_30403&gt;Home_Decor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Lamps_&amp;_Light_Fixtures_30403&gt;Home_Décor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Large_Appliances_30200&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Light_Bulbs_30506&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Living_Room_30306&gt;Furniture_30300&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Mattress_Pads_&amp;_Toppers_30205&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Microwaves_30117&gt;Large_Appliances_30114&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Mixers_&amp;_Accessories_30108&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Nursery_30307&gt;Furniture_30300&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Other_30113&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Other_30210&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Other_30308&gt;Furniture_30300&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Other_30405&gt;Home_Decor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Other_30405&gt;Home_Décor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Other_30517&gt;Tools_30510&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Other_30518&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Other_30613&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Other_30705&gt;Patio_&amp;_Garden_30700&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Other_31000&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Paint_30507&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Pet_Supplies_30800&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Pillows_&amp;_Protectors_30206&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Plumbing_&amp;_Fixing_30508&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Power_Tool_Accessories_30515&gt;Tools_30510&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Power_Tools_30511&gt;Tools_30510&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Refrigerators_30118&gt;Large_Appliances_30114&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Rugs_30404&gt;Home_Décor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Safety_&amp;_Security_30509&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Serveware_30610&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Sheets_30208&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Shower_Curtains_&amp;_Vanity_30207&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Slow_Cookers_30109&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Storage_&amp;_Cleaning_30900&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Toaster_Ovens_30110&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Toasters_30111&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Tool_Storage_30516&gt;Tools_30510&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Towels_30209&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Vacuums_&amp;_Floor_Care_30119&gt;Large_Appliances_30114&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Wall_Ovens_30120&gt;Large_Appliances_30114&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Washers_&amp;_Dryers_30121&gt;Large_Appliances_30114&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
-    <t>Wine_&amp;_Bar_Tools_30612&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</t>
-  </si>
-  <si>
     <t>ROOT 0</t>
   </si>
   <si>
@@ -446,9 +197,6 @@
     <t>Averages</t>
   </si>
   <si>
-    <t>Food #</t>
-  </si>
-  <si>
     <t>Baby &amp; Kids Clothes</t>
   </si>
   <si>
@@ -458,13 +206,43 @@
     <t>Women's Clothing</t>
   </si>
   <si>
-    <t>Other Clothing #</t>
-  </si>
-  <si>
     <t>Baby &amp; Kids Clothing</t>
   </si>
   <si>
-    <t>divergence from uniform</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>* Food</t>
+  </si>
+  <si>
+    <t>* Other Clothing</t>
+  </si>
+  <si>
+    <t>KL(Emp|Unif)</t>
+  </si>
+  <si>
+    <t>Branches</t>
+  </si>
+  <si>
+    <t>Instances</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Pearson</t>
+  </si>
+  <si>
+    <t>LogReg ElasticNet (OvA)</t>
+  </si>
+  <si>
+    <t>LogReg L1 (OvO)</t>
+  </si>
+  <si>
+    <t>CNN w/ pretraining</t>
   </si>
 </sst>
 </file>
@@ -539,7 +317,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="684">
+  <cellStyleXfs count="738">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1224,8 +1002,62 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1236,11 +1068,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="684">
+  <cellStyles count="738">
     <cellStyle name="Comma 2" xfId="95"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1583,6 +1412,33 @@
     <cellStyle name="Followed Hyperlink" xfId="679" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="681" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="683" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="685" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="687" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="689" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="691" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="693" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="695" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="697" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="699" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="701" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="703" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="705" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="707" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="709" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="711" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="713" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="715" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="717" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="719" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="721" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="723" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="725" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="727" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="729" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="731" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="733" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="735" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="737" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1924,6 +1780,33 @@
     <cellStyle name="Hyperlink" xfId="678" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="680" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="682" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="684" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="686" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="688" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="690" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="692" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="694" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="696" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="698" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="700" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="702" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="704" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="706" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="708" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="710" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="712" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="714" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="716" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="718" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="720" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="722" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="724" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="726" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="728" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="730" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="732" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="734" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="736" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1952,13 +1835,32 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
+      <c14:style val="133"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="18"/>
+      <c:style val="33"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>KL (Empirical | Uniform)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
@@ -1966,10 +1868,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0852755318336886"/>
-          <c:y val="0.0338381849996023"/>
-          <c:w val="0.698144713096724"/>
-          <c:h val="0.361849001829317"/>
+          <c:x val="0.127428104505805"/>
+          <c:y val="0.131581025776033"/>
+          <c:w val="0.743365821650342"/>
+          <c:h val="0.402536438264366"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1979,31 +1881,30 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DatasetStats!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KL(Emp|Unif)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="40000"/>
-                    <a:lumOff val="60000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-              <a:tileRect/>
-            </a:gradFill>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>DatasetStats!$C$2:$C$18</c:f>
+              <c:f>DatasetStats!$B$3:$B$17</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>Toys</c:v>
                 </c:pt>
@@ -2041,79 +1942,67 @@
                   <c:v>Baby Products</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Food #</c:v>
+                  <c:v>Baby &amp; Kids Clothes</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Baby &amp; Kids Clothes</c:v>
+                  <c:v>Men's Clothing</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Men's Clothing</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>Women's Clothing</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Other Clothing #</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DatasetStats!$D$2:$D$18</c:f>
+              <c:f>DatasetStats!$C$3:$C$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2.233634E6</c:v>
+                  <c:v>0.200090194089776</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0792816E7</c:v>
+                  <c:v>1.0849848064738</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.013154E6</c:v>
+                  <c:v>0.949948309272575</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.424909E6</c:v>
+                  <c:v>1.23734650060732</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.247092E6</c:v>
+                  <c:v>0.340633094761032</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.383758E6</c:v>
+                  <c:v>1.14654803267585</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0271628E7</c:v>
+                  <c:v>0.961943529071928</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.40793E6</c:v>
+                  <c:v>0.292339437182142</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.974104E6</c:v>
+                  <c:v>0.886034519575576</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.317257E6</c:v>
+                  <c:v>0.794793309848037</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.417114E6</c:v>
+                  <c:v>0.300472545444773</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>282650.0</c:v>
+                  <c:v>0.365184235852218</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.556702E6</c:v>
+                  <c:v>0.522709938345901</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>624913.0</c:v>
+                  <c:v>0.766064661949078</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.469219E6</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.672169E6</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>143426.0</c:v>
+                  <c:v>0.878197488705783</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2128,11 +2017,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2036944920"/>
-        <c:axId val="-2036955192"/>
+        <c:axId val="-1983282408"/>
+        <c:axId val="-2034004088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2036944920"/>
+        <c:axId val="-1983282408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2142,34 +2031,27 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="bg1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
           <a:effectLst>
             <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-              <a:srgbClr val="000000">
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
                 <a:alpha val="43000"/>
-              </a:srgbClr>
+              </a:schemeClr>
             </a:outerShdw>
           </a:effectLst>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr lIns="2">
-            <a:spAutoFit/>
-          </a:bodyPr>
+          <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1200" baseline="0"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2036955192"/>
+        <c:crossAx val="-2034004088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2177,7 +2059,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2036955192"/>
+        <c:axId val="-2034004088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2185,45 +2067,22 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="0" cmpd="sng">
-              <a:prstDash val="sysDash"/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:effectLst>
-            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="43000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr lIns="2">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-2036944920"/>
+        <c:crossAx val="-1983282408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:dispUnits>
-          <c:builtInUnit val="millions"/>
-          <c:dispUnitsLbl>
-            <c:layout/>
-          </c:dispUnitsLbl>
-        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -2245,16 +2104,45 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="116"/>
+      <c14:style val="136"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="16"/>
+      <c:style val="36"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of Branches</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0957347322201347"/>
+          <c:y val="0.122315392740542"/>
+          <c:w val="0.728907480314961"/>
+          <c:h val="0.363321730362973"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -2262,499 +2150,129 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>DatasetStats!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Branches</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>DatasetStats!$C$26:$C$104</c:f>
+              <c:f>DatasetStats!$B$3:$B$17</c:f>
               <c:strCache>
-                <c:ptCount val="79"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>Air_Conditioners_30501&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
+                  <c:v>Toys</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Arts_Crafts_&amp;_Sewing_30401&gt;Home_Decor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
+                  <c:v>Home Furniture &amp; Patio</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Arts_Crafts_&amp;_Sewing_30401&gt;Home_Décor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
+                  <c:v>Jewelry &amp; Watches</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Bar_&amp;_Wine_accessories_30601&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
+                  <c:v>Bag Handbags &amp; Accessories</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Bath_Rugs_&amp;_Mats_30202&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
+                  <c:v>Health Beauty &amp; Fragrance</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Bathroom_Accessories_30201&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
+                  <c:v>Shoes</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Bedroom_&amp;_Mattresses_30203&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
+                  <c:v>Electronics &amp; Computers</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Bedroom_30301&gt;Furniture_30300&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
+                  <c:v>Office</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Blankets_&amp;_Throws_30204&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
+                  <c:v>Sports &amp; Fitness</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Building_Supplies_30513&gt;Tools_30510&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
+                  <c:v>Automotive</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Coffee_Makers_30102&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
+                  <c:v>Industrial</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Cooking_Utensils_&amp;_Tools_30603&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
+                  <c:v>Baby Products</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Cookware_&amp;_Bakeware_30604&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
+                  <c:v>Baby &amp; Kids Clothes</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Cutlery_&amp;_Knives_30605&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
+                  <c:v>Men's Clothing</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Deep_Fryers_30104&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Dishwashers_30115&gt;Large_Appliances_30114&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Drinkware_&amp;_Glassware_30607&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Décor_30704&gt;Patio_&amp;_Garden_30700&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Fine_Art_30402&gt;Home_Décor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Flatware_&amp;_Silverware_30608&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Food_Processors_30105&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Food_Storage_30609&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Freezers_&amp;_Ice_Makers_30116&gt;Large_Appliances_30114&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Furniture_30703&gt;Patio_&amp;_Garden_30700&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Game_Room_&amp;_Bar_30302&gt;Furniture_30300&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Gardening_&amp;_Lawn_Care_30701&gt;Patio_&amp;_Garden_30700&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Griddles_&amp;_Grills_30106&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Grill_&amp;_Outdoors_Cooking_30702&gt;Patio_&amp;_Garden_30700&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>Hand_Tools_30514&gt;Tools_30510&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Hardware_30504&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Heating_Cooling_&amp;_Air_Quality_30505&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Home_Décor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Home_Office_30303&gt;Furniture_30300&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Juicers_&amp;_Blenders_30107&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Kids'_Room_30304&gt;Furniture_30300&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Kitchen_&amp;_Dining_30305&gt;Furniture_30300&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Kitchen_Gadgets_30606&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Lamps_&amp;_Light_Fixtures_30403&gt;Home_Decor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>Lamps_&amp;_Light_Fixtures_30403&gt;Home_Décor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Large_Appliances_30200&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Light_Bulbs_30506&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Living_Room_30306&gt;Furniture_30300&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Mattress_Pads_&amp;_Toppers_30205&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>Microwaves_30117&gt;Large_Appliances_30114&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Mixers_&amp;_Accessories_30108&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Nursery_30307&gt;Furniture_30300&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>Other_30113&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>Other_30210&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>Other_30308&gt;Furniture_30300&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>Other_30405&gt;Home_Decor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>Other_30405&gt;Home_Décor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>Other_30517&gt;Tools_30510&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>Other_30518&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>Other_30613&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>Other_30705&gt;Patio_&amp;_Garden_30700&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>Other_31000&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>Paint_30507&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>Pet_Supplies_30800&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>Pillows_&amp;_Protectors_30206&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>Plumbing_&amp;_Fixing_30508&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>Power_Tool_Accessories_30515&gt;Tools_30510&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>Power_Tools_30511&gt;Tools_30510&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>Refrigerators_30118&gt;Large_Appliances_30114&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>Rugs_30404&gt;Home_Décor_30400&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>Safety_&amp;_Security_30509&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>Serveware_30610&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>Sheets_30208&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>Shower_Curtains_&amp;_Vanity_30207&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>Slow_Cookers_30109&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>Storage_&amp;_Cleaning_30900&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>Toaster_Ovens_30110&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>Toasters_30111&gt;Small_Appliances_30101&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>Tool_Storage_30516&gt;Tools_30510&gt;Home_Improvement_&amp;_Tools_30500&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>Towels_30209&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>Vacuums_&amp;_Floor_Care_30119&gt;Large_Appliances_30114&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>Wall_Ovens_30120&gt;Large_Appliances_30114&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>Washers_&amp;_Dryers_30121&gt;Large_Appliances_30114&gt;Appliances_30100&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>Wine_&amp;_Bar_Tools_30612&gt;Kitchen_&amp;_Dining_30600&gt;Home_Furniture_&amp;_Patio_30000&gt;ROOT_0</c:v>
+                  <c:v>Women's Clothing</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DatasetStats!$D$26:$D$104</c:f>
+              <c:f>DatasetStats!$D$3:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="79"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>34138.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>79.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>421420.0</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16460.0</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19843.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>105768.0</c:v>
+                  <c:v>55.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32491.0</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>160191.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>99472.0</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>170614.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11236.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13696.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>91107.0</c:v>
+                  <c:v>62.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17944.0</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2028.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5042.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>39171.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>138552.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>215525.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>15846.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2379.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2144.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3409.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>248499.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>102314.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>191955.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1333.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>42335.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>214703.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.050686E6</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>109343.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>13331.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>22731.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>9547.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>27914.0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>108557.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>45803.0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>1.587758E6</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>11185.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>61247.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>218377.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>11368.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>5908.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>3836.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>7743.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>17934.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>11786.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>119365.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>592718.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>30115.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>1.464418E6</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>49020.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>128699.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>3326.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>303640.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>186262.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>95228.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>330632.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>218970.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>37824.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>19950.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>687016.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>108684.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>107540.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>142233.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>24735.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>3217.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>236007.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>1641.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>3630.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>41972.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>26322.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>15678.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>44058.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>8037.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>17192.0</c:v>
+                  <c:v>63.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2769,26 +2287,41 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2037047384"/>
-        <c:axId val="-2037050024"/>
+        <c:axId val="-2033490888"/>
+        <c:axId val="-1983242008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2037047384"/>
+        <c:axId val="-2033490888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+                <a:alpha val="43000"/>
+              </a:schemeClr>
+            </a:outerShdw>
+          </a:effectLst>
         </c:spPr>
-        <c:crossAx val="-2037050024"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1983242008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2796,37 +2329,32 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2037050024"/>
+        <c:axId val="-1983242008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="80.0"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="-2037047384"/>
+        <c:crossAx val="-2033490888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:dispUnits>
-          <c:builtInUnit val="millions"/>
-          <c:dispUnitsLbl>
-            <c:layout/>
-          </c:dispUnitsLbl>
-        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -2862,10 +2390,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0636516695255613"/>
-          <c:y val="0.070631970260223"/>
-          <c:w val="0.589784032901399"/>
-          <c:h val="0.45104557562275"/>
+          <c:x val="0.0901651790138043"/>
+          <c:y val="0.125704439119023"/>
+          <c:w val="0.554934103711383"/>
+          <c:h val="0.372784662786717"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3028,7 +2556,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Logistic with ElasticNet (one vs all)</c:v>
+                  <c:v>LogReg ElasticNet (OvA)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3167,7 +2695,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Logistic with L1 (one vs one)</c:v>
+                  <c:v>LogReg L1 (OvO)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3432,7 +2960,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CNN</c:v>
+                  <c:v>CNN w/ pretraining</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3516,49 +3044,49 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>100.0</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100.0</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100.0</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100.0</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100.0</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100.0</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100.0</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100.0</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>100.0</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>100.0</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>100.0</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>100.0</c:v>
+                  <c:v>92.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3575,11 +3103,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2036618216"/>
-        <c:axId val="-2036875608"/>
+        <c:axId val="-1983593768"/>
+        <c:axId val="-2033320552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2036618216"/>
+        <c:axId val="-1983593768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3591,9 +3119,11 @@
         <c:spPr>
           <a:effectLst>
             <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-              <a:srgbClr val="000000">
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
                 <a:alpha val="43000"/>
-              </a:srgbClr>
+              </a:schemeClr>
             </a:outerShdw>
           </a:effectLst>
         </c:spPr>
@@ -3609,7 +3139,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2036875608"/>
+        <c:crossAx val="-2033320552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3617,7 +3147,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2036875608"/>
+        <c:axId val="-2033320552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3644,9 +3174,11 @@
         <c:spPr>
           <a:effectLst>
             <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-              <a:srgbClr val="000000">
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
                 <a:alpha val="43000"/>
-              </a:srgbClr>
+              </a:schemeClr>
             </a:outerShdw>
           </a:effectLst>
         </c:spPr>
@@ -3660,22 +3192,22 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2036618216"/>
+        <c:crossAx val="-1983593768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="t"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.688791403499393"/>
-          <c:y val="0.0291572299045658"/>
-          <c:w val="0.309268732291102"/>
-          <c:h val="0.568851729222893"/>
+          <c:x val="0.0964665259049782"/>
+          <c:y val="0.00869565217391304"/>
+          <c:w val="0.551500484027106"/>
+          <c:h val="0.120285518657994"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3706,21 +3238,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3736,21 +3270,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3772,15 +3308,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>184150</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4124,1024 +3660,702 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R104"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P44" sqref="P44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="40.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="1">
+        <v>20000</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.20009019408977599</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>2233634</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="1">
+        <v>30000</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.0849848064737999</v>
+      </c>
+      <c r="D4">
+        <v>79</v>
+      </c>
+      <c r="E4">
+        <v>10792816</v>
+      </c>
+      <c r="P4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4">
+        <v>2233634</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="1">
+        <v>40000</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.94994830927257501</v>
+      </c>
+      <c r="D5">
+        <v>36</v>
+      </c>
+      <c r="E5">
+        <v>3013241</v>
+      </c>
+      <c r="P5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q5">
+        <v>10792816</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="1">
+        <v>70000</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.2373465006073201</v>
+      </c>
+      <c r="D6">
+        <v>51</v>
+      </c>
+      <c r="E6">
+        <v>1425157</v>
+      </c>
+      <c r="P6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6">
+        <v>3013154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="1">
+        <v>80000</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.34063309476103198</v>
+      </c>
+      <c r="D7">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <v>5247093</v>
+      </c>
+      <c r="P7" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="Q7">
+        <v>1424909</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="1">
+        <v>90000</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.1465480326758499</v>
+      </c>
+      <c r="D8">
+        <v>55</v>
+      </c>
+      <c r="E8">
+        <v>2383758</v>
+      </c>
+      <c r="P8" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q8">
+        <v>5247092</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.96194352907192804</v>
+      </c>
+      <c r="D9">
+        <v>59</v>
+      </c>
+      <c r="E9">
+        <v>10271628</v>
+      </c>
+      <c r="P9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9">
+        <v>2383758</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="1">
+        <v>110000</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.292339437182142</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>3407930</v>
+      </c>
+      <c r="P10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q10">
+        <v>10271628</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="1">
+        <v>120000</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.886034519575576</v>
+      </c>
+      <c r="D11">
+        <v>40</v>
+      </c>
+      <c r="E11">
+        <v>1974104</v>
+      </c>
+      <c r="P11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q11">
+        <v>3407930</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="1">
+        <v>130000</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.79479330984803698</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>7317257</v>
+      </c>
+      <c r="P12" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q12">
+        <v>1974104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="1">
+        <v>140000</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.30047254544477298</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>5417114</v>
+      </c>
+      <c r="P13" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q13">
+        <v>7317257</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="1">
+        <v>180000</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.36518423585221799</v>
+      </c>
+      <c r="D14">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>282650</v>
+      </c>
+      <c r="P14" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q14">
+        <v>5417114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="1">
+        <v>210000</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.52270993834590096</v>
+      </c>
+      <c r="D15">
+        <v>62</v>
+      </c>
+      <c r="E15">
+        <v>624913</v>
+      </c>
+      <c r="P15" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q15">
+        <v>282650</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="1">
+        <v>250000</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.76606466194907796</v>
+      </c>
+      <c r="D16">
+        <v>41</v>
+      </c>
+      <c r="E16">
+        <v>1469219</v>
+      </c>
+      <c r="P16" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q16">
+        <v>1556702</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="1">
+        <v>260000</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.87819748870578296</v>
+      </c>
+      <c r="D17">
+        <v>63</v>
+      </c>
+      <c r="E17">
+        <v>2672169</v>
+      </c>
+      <c r="P17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q17">
+        <v>624913</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="E18">
+        <f>SUM(E3:E17)</f>
+        <v>58532683</v>
+      </c>
+      <c r="P18" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q18">
+        <v>1469219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="6">
+        <f>AVERAGE(C3:C17)</f>
+        <v>0.71515270692371946</v>
+      </c>
+      <c r="D19" s="2">
+        <f>AVERAGE(D3:D17)</f>
+        <v>38.06666666666667</v>
+      </c>
+      <c r="E19">
+        <f>AVERAGE(E3:E17)</f>
+        <v>3902178.8666666667</v>
+      </c>
+      <c r="P19" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q19">
+        <v>2672169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20">
+        <f>PEARSON(D3:D17,E3:E17)</f>
+        <v>0.20935700047565201</v>
+      </c>
+      <c r="P20" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q20">
+        <v>143426</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D30" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
-      <c r="A2" s="1" t="s">
+    <row r="31" spans="1:17">
+      <c r="A31" s="1">
+        <v>20000</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31">
+        <v>2233634</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32" s="1">
+        <v>30000</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32">
+        <v>10792816</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1">
+        <v>40000</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33">
+        <v>3013154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
+        <v>70000</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34">
+        <v>1424909</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
+        <v>80000</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C35" t="s">
         <v>44</v>
       </c>
-      <c r="D2">
-        <v>2233634</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="A3" s="1" t="s">
+      <c r="D35">
+        <v>5247092</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
+        <v>90000</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C36" t="s">
         <v>45</v>
       </c>
-      <c r="D3">
-        <v>10792816</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R3">
-        <v>2233634</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" s="1" t="s">
+      <c r="D36">
+        <v>2383758</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C37" t="s">
         <v>46</v>
       </c>
-      <c r="D4">
-        <v>3013154</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>11</v>
-      </c>
-      <c r="R4">
-        <v>10792816</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="A5" s="1" t="s">
+      <c r="D37">
+        <v>10271628</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>110000</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C38" t="s">
         <v>47</v>
       </c>
-      <c r="D5">
-        <v>1424909</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>12</v>
-      </c>
-      <c r="R5">
-        <v>3013154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="A6" s="1" t="s">
+      <c r="D38">
+        <v>3407930</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
+        <v>120000</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="C39" t="s">
         <v>48</v>
       </c>
-      <c r="D6">
-        <v>5247092</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>13</v>
-      </c>
-      <c r="R6">
-        <v>1424909</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" s="1" t="s">
+      <c r="D39">
+        <v>1974104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
+        <v>130000</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C40" t="s">
         <v>49</v>
       </c>
-      <c r="D7">
-        <v>2383758</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>14</v>
-      </c>
-      <c r="R7">
-        <v>5247092</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
-      <c r="A8" s="1" t="s">
+      <c r="D40">
+        <v>7317257</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
+        <v>140000</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C41" t="s">
         <v>50</v>
       </c>
-      <c r="D8">
-        <v>10271628</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>15</v>
-      </c>
-      <c r="R8">
-        <v>2383758</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="A9" s="1" t="s">
+      <c r="D41">
+        <v>5417114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>180000</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="C42" t="s">
         <v>51</v>
       </c>
-      <c r="D9">
-        <v>3407930</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>16</v>
-      </c>
-      <c r="R9">
-        <v>10271628</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="A10" s="1" t="s">
+      <c r="D42">
+        <v>282650</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>190000</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10">
-        <v>1974104</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>17</v>
-      </c>
-      <c r="R10">
-        <v>3407930</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="A11" s="1" t="s">
+      <c r="C43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43">
+        <v>1556702</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>210000</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11">
-        <v>7317257</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>18</v>
-      </c>
-      <c r="R11">
-        <v>1974104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="A12" s="1" t="s">
+      <c r="C44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44">
+        <v>624913</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>250000</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12">
-        <v>5417114</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R12">
-        <v>7317257</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="A13" s="1" t="s">
+      <c r="C45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45">
+        <v>1469219</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>260000</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13">
-        <v>282650</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>20</v>
-      </c>
-      <c r="R13">
-        <v>5417114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="1" t="s">
+      <c r="C46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46">
+        <v>2672169</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>270000</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" t="s">
-        <v>141</v>
-      </c>
-      <c r="D14">
-        <v>1556702</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>21</v>
-      </c>
-      <c r="R14">
-        <v>282650</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="A15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>142</v>
-      </c>
-      <c r="D15">
-        <v>624913</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>22</v>
-      </c>
-      <c r="R15">
-        <v>1556702</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="A16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>143</v>
-      </c>
-      <c r="D16">
-        <v>1469219</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>23</v>
-      </c>
-      <c r="R16">
-        <v>624913</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
-      <c r="A17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>144</v>
-      </c>
-      <c r="D17">
-        <v>2672169</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>24</v>
-      </c>
-      <c r="R17">
-        <v>1469219</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18">
-      <c r="A18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" t="s">
-        <v>145</v>
-      </c>
-      <c r="D18">
+      <c r="C47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47">
         <v>143426</v>
       </c>
-      <c r="Q18" t="s">
-        <v>25</v>
-      </c>
-      <c r="R18">
-        <v>2672169</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="Q19" t="s">
-        <v>26</v>
-      </c>
-      <c r="R19">
-        <v>143426</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:18">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:18">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:18">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:18">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-    </row>
-    <row r="26" spans="1:18">
-      <c r="C26" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26">
-        <v>34138</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18">
-      <c r="C27" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18">
-      <c r="C28" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28">
-        <v>421420</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18">
-      <c r="C29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29">
-        <v>16460</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18">
-      <c r="C30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30">
-        <v>19843</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18">
-      <c r="C31" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31">
-        <v>105768</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18">
-      <c r="C32" t="s">
-        <v>65</v>
-      </c>
-      <c r="D32">
-        <v>32491</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4">
-      <c r="C33" t="s">
-        <v>66</v>
-      </c>
-      <c r="D33">
-        <v>160191</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4">
-      <c r="C34" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34">
-        <v>99472</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4">
-      <c r="C35" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35">
-        <v>170614</v>
-      </c>
-    </row>
-    <row r="36" spans="3:4">
-      <c r="C36" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36">
-        <v>11236</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4">
-      <c r="C37" t="s">
-        <v>70</v>
-      </c>
-      <c r="D37">
-        <v>13696</v>
-      </c>
-    </row>
-    <row r="38" spans="3:4">
-      <c r="C38" t="s">
-        <v>71</v>
-      </c>
-      <c r="D38">
-        <v>91107</v>
-      </c>
-    </row>
-    <row r="39" spans="3:4">
-      <c r="C39" t="s">
-        <v>72</v>
-      </c>
-      <c r="D39">
-        <v>17944</v>
-      </c>
-    </row>
-    <row r="40" spans="3:4">
-      <c r="C40" t="s">
-        <v>73</v>
-      </c>
-      <c r="D40">
-        <v>2028</v>
-      </c>
-    </row>
-    <row r="41" spans="3:4">
-      <c r="C41" t="s">
-        <v>74</v>
-      </c>
-      <c r="D41">
-        <v>5042</v>
-      </c>
-    </row>
-    <row r="42" spans="3:4">
-      <c r="C42" t="s">
-        <v>75</v>
-      </c>
-      <c r="D42">
-        <v>39171</v>
-      </c>
-    </row>
-    <row r="43" spans="3:4">
-      <c r="C43" t="s">
-        <v>76</v>
-      </c>
-      <c r="D43">
-        <v>138552</v>
-      </c>
-    </row>
-    <row r="44" spans="3:4">
-      <c r="C44" t="s">
-        <v>77</v>
-      </c>
-      <c r="D44">
-        <v>215525</v>
-      </c>
-    </row>
-    <row r="45" spans="3:4">
-      <c r="C45" t="s">
-        <v>78</v>
-      </c>
-      <c r="D45">
-        <v>15846</v>
-      </c>
-    </row>
-    <row r="46" spans="3:4">
-      <c r="C46" t="s">
-        <v>79</v>
-      </c>
-      <c r="D46">
-        <v>2379</v>
-      </c>
-    </row>
-    <row r="47" spans="3:4">
-      <c r="C47" t="s">
-        <v>80</v>
-      </c>
-      <c r="D47">
-        <v>2144</v>
-      </c>
-    </row>
-    <row r="48" spans="3:4">
-      <c r="C48" t="s">
-        <v>81</v>
-      </c>
-      <c r="D48">
-        <v>3409</v>
-      </c>
-    </row>
-    <row r="49" spans="3:4">
-      <c r="C49" t="s">
-        <v>82</v>
-      </c>
-      <c r="D49">
-        <v>248499</v>
-      </c>
-    </row>
-    <row r="50" spans="3:4">
-      <c r="C50" t="s">
-        <v>83</v>
-      </c>
-      <c r="D50">
-        <v>102314</v>
-      </c>
-    </row>
-    <row r="51" spans="3:4">
-      <c r="C51" t="s">
-        <v>84</v>
-      </c>
-      <c r="D51">
-        <v>191955</v>
-      </c>
-    </row>
-    <row r="52" spans="3:4">
-      <c r="C52" t="s">
-        <v>85</v>
-      </c>
-      <c r="D52">
-        <v>1333</v>
-      </c>
-    </row>
-    <row r="53" spans="3:4">
-      <c r="C53" t="s">
-        <v>86</v>
-      </c>
-      <c r="D53">
-        <v>42335</v>
-      </c>
-    </row>
-    <row r="54" spans="3:4">
-      <c r="C54" t="s">
-        <v>87</v>
-      </c>
-      <c r="D54">
-        <v>214703</v>
-      </c>
-    </row>
-    <row r="55" spans="3:4">
-      <c r="C55" t="s">
-        <v>88</v>
-      </c>
-      <c r="D55">
-        <v>1050686</v>
-      </c>
-    </row>
-    <row r="56" spans="3:4">
-      <c r="C56" t="s">
-        <v>89</v>
-      </c>
-      <c r="D56">
-        <v>109343</v>
-      </c>
-    </row>
-    <row r="57" spans="3:4">
-      <c r="C57" t="s">
-        <v>90</v>
-      </c>
-      <c r="D57">
-        <v>13331</v>
-      </c>
-    </row>
-    <row r="58" spans="3:4">
-      <c r="C58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D58">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="59" spans="3:4">
-      <c r="C59" t="s">
-        <v>92</v>
-      </c>
-      <c r="D59">
-        <v>22731</v>
-      </c>
-    </row>
-    <row r="60" spans="3:4">
-      <c r="C60" t="s">
-        <v>93</v>
-      </c>
-      <c r="D60">
-        <v>9547</v>
-      </c>
-    </row>
-    <row r="61" spans="3:4">
-      <c r="C61" t="s">
-        <v>94</v>
-      </c>
-      <c r="D61">
-        <v>27914</v>
-      </c>
-    </row>
-    <row r="62" spans="3:4">
-      <c r="C62" t="s">
-        <v>95</v>
-      </c>
-      <c r="D62">
-        <v>108557</v>
-      </c>
-    </row>
-    <row r="63" spans="3:4">
-      <c r="C63" t="s">
-        <v>96</v>
-      </c>
-      <c r="D63">
-        <v>45803</v>
-      </c>
-    </row>
-    <row r="64" spans="3:4">
-      <c r="C64" t="s">
-        <v>97</v>
-      </c>
-      <c r="D64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="3:4">
-      <c r="C65" t="s">
-        <v>98</v>
-      </c>
-      <c r="D65">
-        <v>1587758</v>
-      </c>
-    </row>
-    <row r="66" spans="3:4">
-      <c r="C66" t="s">
-        <v>99</v>
-      </c>
-      <c r="D66">
-        <v>11185</v>
-      </c>
-    </row>
-    <row r="67" spans="3:4">
-      <c r="C67" t="s">
-        <v>100</v>
-      </c>
-      <c r="D67">
-        <v>61247</v>
-      </c>
-    </row>
-    <row r="68" spans="3:4">
-      <c r="C68" t="s">
-        <v>101</v>
-      </c>
-      <c r="D68">
-        <v>218377</v>
-      </c>
-    </row>
-    <row r="69" spans="3:4">
-      <c r="C69" t="s">
-        <v>102</v>
-      </c>
-      <c r="D69">
-        <v>11368</v>
-      </c>
-    </row>
-    <row r="70" spans="3:4">
-      <c r="C70" t="s">
-        <v>103</v>
-      </c>
-      <c r="D70">
-        <v>5908</v>
-      </c>
-    </row>
-    <row r="71" spans="3:4">
-      <c r="C71" t="s">
-        <v>104</v>
-      </c>
-      <c r="D71">
-        <v>3836</v>
-      </c>
-    </row>
-    <row r="72" spans="3:4">
-      <c r="C72" t="s">
-        <v>105</v>
-      </c>
-      <c r="D72">
-        <v>7743</v>
-      </c>
-    </row>
-    <row r="73" spans="3:4">
-      <c r="C73" t="s">
-        <v>106</v>
-      </c>
-      <c r="D73">
-        <v>17934</v>
-      </c>
-    </row>
-    <row r="74" spans="3:4">
-      <c r="C74" t="s">
-        <v>107</v>
-      </c>
-      <c r="D74">
-        <v>11786</v>
-      </c>
-    </row>
-    <row r="75" spans="3:4">
-      <c r="C75" t="s">
-        <v>108</v>
-      </c>
-      <c r="D75">
-        <v>119365</v>
-      </c>
-    </row>
-    <row r="76" spans="3:4">
-      <c r="C76" t="s">
-        <v>109</v>
-      </c>
-      <c r="D76">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="3:4">
-      <c r="C77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D77">
-        <v>592718</v>
-      </c>
-    </row>
-    <row r="78" spans="3:4">
-      <c r="C78" t="s">
-        <v>111</v>
-      </c>
-      <c r="D78">
-        <v>30115</v>
-      </c>
-    </row>
-    <row r="79" spans="3:4">
-      <c r="C79" t="s">
-        <v>112</v>
-      </c>
-      <c r="D79">
-        <v>1464418</v>
-      </c>
-    </row>
-    <row r="80" spans="3:4">
-      <c r="C80" t="s">
-        <v>113</v>
-      </c>
-      <c r="D80">
-        <v>49020</v>
-      </c>
-    </row>
-    <row r="81" spans="3:4">
-      <c r="C81" t="s">
-        <v>114</v>
-      </c>
-      <c r="D81">
-        <v>128699</v>
-      </c>
-    </row>
-    <row r="82" spans="3:4">
-      <c r="C82" t="s">
-        <v>115</v>
-      </c>
-      <c r="D82">
-        <v>3326</v>
-      </c>
-    </row>
-    <row r="83" spans="3:4">
-      <c r="C83" t="s">
-        <v>116</v>
-      </c>
-      <c r="D83">
-        <v>303640</v>
-      </c>
-    </row>
-    <row r="84" spans="3:4">
-      <c r="C84" t="s">
-        <v>117</v>
-      </c>
-      <c r="D84">
-        <v>186262</v>
-      </c>
-    </row>
-    <row r="85" spans="3:4">
-      <c r="C85" t="s">
-        <v>118</v>
-      </c>
-      <c r="D85">
-        <v>95228</v>
-      </c>
-    </row>
-    <row r="86" spans="3:4">
-      <c r="C86" t="s">
-        <v>119</v>
-      </c>
-      <c r="D86">
-        <v>330632</v>
-      </c>
-    </row>
-    <row r="87" spans="3:4">
-      <c r="C87" t="s">
-        <v>120</v>
-      </c>
-      <c r="D87">
-        <v>218970</v>
-      </c>
-    </row>
-    <row r="88" spans="3:4">
-      <c r="C88" t="s">
-        <v>121</v>
-      </c>
-      <c r="D88">
-        <v>37824</v>
-      </c>
-    </row>
-    <row r="89" spans="3:4">
-      <c r="C89" t="s">
-        <v>122</v>
-      </c>
-      <c r="D89">
-        <v>19950</v>
-      </c>
-    </row>
-    <row r="90" spans="3:4">
-      <c r="C90" t="s">
-        <v>123</v>
-      </c>
-      <c r="D90">
-        <v>687016</v>
-      </c>
-    </row>
-    <row r="91" spans="3:4">
-      <c r="C91" t="s">
-        <v>124</v>
-      </c>
-      <c r="D91">
-        <v>108684</v>
-      </c>
-    </row>
-    <row r="92" spans="3:4">
-      <c r="C92" t="s">
-        <v>125</v>
-      </c>
-      <c r="D92">
-        <v>107540</v>
-      </c>
-    </row>
-    <row r="93" spans="3:4">
-      <c r="C93" t="s">
-        <v>126</v>
-      </c>
-      <c r="D93">
-        <v>142233</v>
-      </c>
-    </row>
-    <row r="94" spans="3:4">
-      <c r="C94" t="s">
-        <v>127</v>
-      </c>
-      <c r="D94">
-        <v>24735</v>
-      </c>
-    </row>
-    <row r="95" spans="3:4">
-      <c r="C95" t="s">
-        <v>128</v>
-      </c>
-      <c r="D95">
-        <v>3217</v>
-      </c>
-    </row>
-    <row r="96" spans="3:4">
-      <c r="C96" t="s">
-        <v>129</v>
-      </c>
-      <c r="D96">
-        <v>236007</v>
-      </c>
-    </row>
-    <row r="97" spans="3:4">
-      <c r="C97" t="s">
-        <v>130</v>
-      </c>
-      <c r="D97">
-        <v>1641</v>
-      </c>
-    </row>
-    <row r="98" spans="3:4">
-      <c r="C98" t="s">
-        <v>131</v>
-      </c>
-      <c r="D98">
-        <v>3630</v>
-      </c>
-    </row>
-    <row r="99" spans="3:4">
-      <c r="C99" t="s">
-        <v>132</v>
-      </c>
-      <c r="D99">
-        <v>41972</v>
-      </c>
-    </row>
-    <row r="100" spans="3:4">
-      <c r="C100" t="s">
-        <v>133</v>
-      </c>
-      <c r="D100">
-        <v>26322</v>
-      </c>
-    </row>
-    <row r="101" spans="3:4">
-      <c r="C101" t="s">
-        <v>134</v>
-      </c>
-      <c r="D101">
-        <v>15678</v>
-      </c>
-    </row>
-    <row r="102" spans="3:4">
-      <c r="C102" t="s">
-        <v>135</v>
-      </c>
-      <c r="D102">
-        <v>44058</v>
-      </c>
-    </row>
-    <row r="103" spans="3:4">
-      <c r="C103" t="s">
-        <v>136</v>
-      </c>
-      <c r="D103">
-        <v>8037</v>
-      </c>
-    </row>
-    <row r="104" spans="3:4">
-      <c r="C104" t="s">
-        <v>137</v>
-      </c>
-      <c r="D104">
-        <v>17192</v>
-      </c>
     </row>
   </sheetData>
+  <sortState ref="F3:I18">
+    <sortCondition ref="F3"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
@@ -5155,23 +4369,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K90"/>
+  <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F17"/>
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
@@ -5186,24 +4403,24 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C3" s="2">
         <v>66.492504999999994</v>
@@ -5218,15 +4435,15 @@
         <v>86.320642119120095</v>
       </c>
       <c r="G3" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2">
         <v>64.820767000000004</v>
@@ -5241,15 +4458,15 @@
         <v>90</v>
       </c>
       <c r="G4" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C5" s="2">
         <v>52.309280000000001</v>
@@ -5264,15 +4481,15 @@
         <v>91.024201633065303</v>
       </c>
       <c r="G5" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C6" s="2">
         <v>70.278749000000005</v>
@@ -5287,15 +4504,15 @@
         <v>90.432399190786796</v>
       </c>
       <c r="G6" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C7" s="2">
         <v>75.048933000000005</v>
@@ -5310,15 +4527,15 @@
         <v>90.882761192694204</v>
       </c>
       <c r="G7" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2">
         <v>58.221629</v>
@@ -5333,15 +4550,15 @@
         <v>77.488465174735197</v>
       </c>
       <c r="G8" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2">
         <v>65.39179</v>
@@ -5356,15 +4573,15 @@
         <v>88.62</v>
       </c>
       <c r="G9" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2">
         <v>77.970467999999997</v>
@@ -5379,15 +4596,15 @@
         <v>94.945618910563695</v>
       </c>
       <c r="G10" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C11" s="2">
         <v>75.028116999999995</v>
@@ -5402,15 +4619,15 @@
         <v>91.334553070973698</v>
       </c>
       <c r="G11" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C12" s="2">
         <v>75.582566999999997</v>
@@ -5425,15 +4642,15 @@
         <v>96.148514988790296</v>
       </c>
       <c r="G12" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C13" s="2">
         <v>76.075856000000002</v>
@@ -5448,15 +4665,15 @@
         <v>95.842222057607799</v>
       </c>
       <c r="G13" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C14" s="2">
         <v>78.287029000000004</v>
@@ -5471,15 +4688,15 @@
         <v>92.799203888301406</v>
       </c>
       <c r="G14" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>61</v>
       </c>
       <c r="C15" s="2">
         <v>57.460093999999998</v>
@@ -5494,15 +4711,15 @@
         <v>88.334653784167202</v>
       </c>
       <c r="G15" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>59</v>
       </c>
       <c r="C16" s="2">
         <v>63.919728999999997</v>
@@ -5517,15 +4734,15 @@
         <v>91.186976647721096</v>
       </c>
       <c r="G16" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>60</v>
       </c>
       <c r="C17" s="2">
         <v>62.385987</v>
@@ -5540,15 +4757,15 @@
         <v>91.850017906641497</v>
       </c>
       <c r="G17" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
-        <v>138</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>56</v>
       </c>
       <c r="C18" s="2">
         <v>72.135182</v>
@@ -5563,7 +4780,7 @@
         <v>93</v>
       </c>
       <c r="G18" s="2">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -5571,25 +4788,32 @@
         <f>AVERAGE(C3:C18)</f>
         <v>68.213042625</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <f>AVERAGE(D3:D18)</f>
         <v>84.288704187499988</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <f>AVERAGE(E3:E18)</f>
         <v>85.013125000000016</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <f>AVERAGE(F3:F18)</f>
         <v>90.638139410323021</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
+      <c r="G19" s="2">
+        <f>AVERAGE(G3:G18)</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11">
       <c r="C27" s="2"/>
@@ -5741,22 +4965,18 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="3:11">
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-    </row>
-    <row r="78" spans="2:6">
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
-      <c r="F78" s="7"/>
+    <row r="77" spans="2:6">
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+    </row>
+    <row r="79" spans="2:6">
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
     </row>
     <row r="80" spans="2:6">
       <c r="C80" s="2"/>
@@ -5776,18 +4996,16 @@
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
     </row>
-    <row r="83" spans="2:6">
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
-      <c r="E83" s="2"/>
-      <c r="F83" s="2"/>
-    </row>
-    <row r="85" spans="2:6">
-      <c r="B85" s="7"/>
-      <c r="C85" s="7"/>
-      <c r="D85" s="7"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
+    <row r="84" spans="2:6">
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+    </row>
+    <row r="86" spans="2:6">
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
     </row>
     <row r="87" spans="2:6">
       <c r="C87" s="2"/>
@@ -5800,20 +5018,15 @@
     <row r="89" spans="2:6">
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
-    </row>
-    <row r="90" spans="2:6">
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
     </row>
   </sheetData>
   <sortState ref="D52:E67">
     <sortCondition ref="D52"/>
   </sortState>
-  <mergeCells count="4">
-    <mergeCell ref="B85:D85"/>
+  <mergeCells count="3">
+    <mergeCell ref="B84:D84"/>
     <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B77:F77"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5828,10 +5041,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5846,650 +5059,660 @@
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>147</v>
+      <c r="I1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B2" s="4">
         <v>66.489999999999995</v>
       </c>
-      <c r="C2" s="4">
-        <v>0.27</v>
+      <c r="C2" s="6">
+        <v>0.20009019408977599</v>
       </c>
       <c r="D2" s="4">
         <v>79.2</v>
       </c>
-      <c r="E2" s="4">
-        <v>0.27</v>
+      <c r="E2" s="6">
+        <v>0.20009019408977599</v>
       </c>
       <c r="F2" s="1">
         <v>79.959999999999994</v>
       </c>
-      <c r="G2" s="4">
-        <v>0.27</v>
+      <c r="G2" s="6">
+        <v>0.20009019408977599</v>
       </c>
       <c r="H2" s="2">
         <v>86.320642119120095</v>
       </c>
-      <c r="I2" s="4">
-        <v>0.27</v>
+      <c r="I2" s="6">
+        <v>0.20009019408977599</v>
       </c>
       <c r="J2" s="4">
-        <v>100</v>
-      </c>
-      <c r="K2" s="4">
-        <v>0.27</v>
+        <v>92</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0.20009019408977599</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B3" s="4">
         <v>64.819999999999993</v>
       </c>
-      <c r="C3" s="4">
-        <v>1.72</v>
+      <c r="C3" s="6">
+        <v>1.0849848064737999</v>
       </c>
       <c r="D3" s="4">
         <v>85.11</v>
       </c>
-      <c r="E3" s="4">
-        <v>1.72</v>
+      <c r="E3" s="6">
+        <v>1.0849848064737999</v>
       </c>
       <c r="F3" s="1">
         <v>86.86</v>
       </c>
-      <c r="G3" s="4">
-        <v>1.72</v>
+      <c r="G3" s="6">
+        <v>1.0849848064737999</v>
       </c>
       <c r="H3" s="2">
         <v>90</v>
       </c>
-      <c r="I3" s="4">
-        <v>1.72</v>
+      <c r="I3" s="6">
+        <v>1.0849848064737999</v>
       </c>
       <c r="J3" s="4">
-        <v>100</v>
-      </c>
-      <c r="K3" s="4">
-        <v>1.72</v>
+        <v>92</v>
+      </c>
+      <c r="K3" s="6">
+        <v>1.0849848064737999</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B4" s="4">
         <v>52.31</v>
       </c>
-      <c r="C4" s="4">
-        <v>2.95</v>
+      <c r="C4" s="6">
+        <v>0.94994830927257501</v>
       </c>
       <c r="D4" s="4">
         <v>81.180000000000007</v>
       </c>
-      <c r="E4" s="4">
-        <v>2.95</v>
+      <c r="E4" s="6">
+        <v>0.94994830927257501</v>
       </c>
       <c r="F4" s="1">
         <v>82.47</v>
       </c>
-      <c r="G4" s="4">
-        <v>2.95</v>
+      <c r="G4" s="6">
+        <v>0.94994830927257501</v>
       </c>
       <c r="H4" s="2">
         <v>91.024201633065303</v>
       </c>
-      <c r="I4" s="4">
-        <v>2.95</v>
+      <c r="I4" s="6">
+        <v>0.94994830927257501</v>
       </c>
       <c r="J4" s="4">
-        <v>100</v>
-      </c>
-      <c r="K4" s="4">
-        <v>2.95</v>
+        <v>92</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0.94994830927257501</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B5" s="4">
         <v>70.28</v>
       </c>
-      <c r="C5" s="4">
-        <v>4.9800000000000004</v>
+      <c r="C5" s="6">
+        <v>1.2373465006073201</v>
       </c>
       <c r="D5" s="4">
         <v>85.09</v>
       </c>
-      <c r="E5" s="4">
-        <v>4.9800000000000004</v>
+      <c r="E5" s="6">
+        <v>1.2373465006073201</v>
       </c>
       <c r="F5" s="1">
         <v>86.26</v>
       </c>
-      <c r="G5" s="4">
-        <v>4.9800000000000004</v>
+      <c r="G5" s="6">
+        <v>1.2373465006073201</v>
       </c>
       <c r="H5" s="2">
         <v>90.432399190786796</v>
       </c>
-      <c r="I5" s="4">
-        <v>4.9800000000000004</v>
+      <c r="I5" s="6">
+        <v>1.2373465006073201</v>
       </c>
       <c r="J5" s="4">
-        <v>100</v>
-      </c>
-      <c r="K5" s="4">
-        <v>4.9800000000000004</v>
+        <v>92</v>
+      </c>
+      <c r="K5" s="6">
+        <v>1.2373465006073201</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B6" s="4">
         <v>75.05</v>
       </c>
-      <c r="C6" s="4">
-        <v>0.8</v>
+      <c r="C6" s="6">
+        <v>0.34063309476103198</v>
       </c>
       <c r="D6" s="4">
         <v>84.42</v>
       </c>
-      <c r="E6" s="4">
-        <v>0.8</v>
+      <c r="E6" s="6">
+        <v>0.34063309476103198</v>
       </c>
       <c r="F6" s="1">
         <v>85.89</v>
       </c>
-      <c r="G6" s="4">
-        <v>0.8</v>
+      <c r="G6" s="6">
+        <v>0.34063309476103198</v>
       </c>
       <c r="H6" s="2">
         <v>90.882761192694204</v>
       </c>
-      <c r="I6" s="4">
-        <v>0.8</v>
+      <c r="I6" s="6">
+        <v>0.34063309476103198</v>
       </c>
       <c r="J6" s="4">
-        <v>100</v>
-      </c>
-      <c r="K6" s="4">
-        <v>0.8</v>
+        <v>92</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0.34063309476103198</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B7" s="4">
         <v>58.22</v>
       </c>
-      <c r="C7" s="4">
-        <v>3.74</v>
+      <c r="C7" s="6">
+        <v>1.1465480326758499</v>
       </c>
       <c r="D7" s="4">
         <v>70.8</v>
       </c>
-      <c r="E7" s="4">
-        <v>3.74</v>
+      <c r="E7" s="6">
+        <v>1.1465480326758499</v>
       </c>
       <c r="F7" s="1">
         <v>72.239999999999995</v>
       </c>
-      <c r="G7" s="4">
-        <v>3.74</v>
+      <c r="G7" s="6">
+        <v>1.1465480326758499</v>
       </c>
       <c r="H7" s="2">
         <v>77.488465174735197</v>
       </c>
-      <c r="I7" s="4">
-        <v>3.74</v>
+      <c r="I7" s="6">
+        <v>1.1465480326758499</v>
       </c>
       <c r="J7" s="4">
-        <v>100</v>
-      </c>
-      <c r="K7" s="4">
-        <v>3.74</v>
+        <v>92</v>
+      </c>
+      <c r="K7" s="6">
+        <v>1.1465480326758499</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B8" s="4">
         <v>65.39</v>
       </c>
-      <c r="C8" s="4">
-        <v>3.13</v>
+      <c r="C8" s="6">
+        <v>0.96194352907192804</v>
       </c>
       <c r="D8" s="4">
         <v>80.930000000000007</v>
       </c>
-      <c r="E8" s="4">
-        <v>3.13</v>
+      <c r="E8" s="6">
+        <v>0.96194352907192804</v>
       </c>
       <c r="F8" s="1">
         <v>82.72</v>
       </c>
-      <c r="G8" s="4">
-        <v>3.13</v>
+      <c r="G8" s="6">
+        <v>0.96194352907192804</v>
       </c>
       <c r="H8" s="2">
         <v>88.62</v>
       </c>
-      <c r="I8" s="4">
-        <v>3.13</v>
+      <c r="I8" s="6">
+        <v>0.96194352907192804</v>
       </c>
       <c r="J8" s="4">
-        <v>100</v>
-      </c>
-      <c r="K8" s="4">
-        <v>3.13</v>
+        <v>92</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.96194352907192804</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B9" s="4">
         <v>77.97</v>
       </c>
-      <c r="C9" s="4">
-        <v>0.45</v>
+      <c r="C9" s="6">
+        <v>0.292339437182142</v>
       </c>
       <c r="D9" s="4">
         <v>90.23</v>
       </c>
-      <c r="E9" s="4">
-        <v>0.45</v>
+      <c r="E9" s="6">
+        <v>0.292339437182142</v>
       </c>
       <c r="F9" s="1">
         <v>90.83</v>
       </c>
-      <c r="G9" s="4">
-        <v>0.45</v>
+      <c r="G9" s="6">
+        <v>0.292339437182142</v>
       </c>
       <c r="H9" s="2">
         <v>94.945618910563695</v>
       </c>
-      <c r="I9" s="4">
-        <v>0.45</v>
+      <c r="I9" s="6">
+        <v>0.292339437182142</v>
       </c>
       <c r="J9" s="4">
-        <v>100</v>
-      </c>
-      <c r="K9" s="4">
-        <v>0.45</v>
+        <v>92</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0.292339437182142</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B10" s="4">
         <v>75.03</v>
       </c>
-      <c r="C10" s="4">
-        <v>2.64</v>
+      <c r="C10" s="6">
+        <v>0.886034519575576</v>
       </c>
       <c r="D10" s="4">
         <v>84.97</v>
       </c>
-      <c r="E10" s="4">
-        <v>2.64</v>
+      <c r="E10" s="6">
+        <v>0.886034519575576</v>
       </c>
       <c r="F10" s="1">
         <v>86.37</v>
       </c>
-      <c r="G10" s="4">
-        <v>2.64</v>
+      <c r="G10" s="6">
+        <v>0.886034519575576</v>
       </c>
       <c r="H10" s="2">
         <v>91.334553070973698</v>
       </c>
-      <c r="I10" s="4">
-        <v>2.64</v>
+      <c r="I10" s="6">
+        <v>0.886034519575576</v>
       </c>
       <c r="J10" s="4">
-        <v>100</v>
-      </c>
-      <c r="K10" s="4">
-        <v>2.64</v>
+        <v>92</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0.886034519575576</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B11" s="4">
         <v>75.58</v>
       </c>
-      <c r="C11" s="4">
-        <v>1.1299999999999999</v>
+      <c r="C11" s="6">
+        <v>0.79479330984803698</v>
       </c>
       <c r="D11" s="4">
         <v>89.41</v>
       </c>
-      <c r="E11" s="4">
-        <v>1.1299999999999999</v>
+      <c r="E11" s="6">
+        <v>0.79479330984803698</v>
       </c>
       <c r="F11" s="1">
         <v>90.28</v>
       </c>
-      <c r="G11" s="4">
-        <v>1.1299999999999999</v>
+      <c r="G11" s="6">
+        <v>0.79479330984803698</v>
       </c>
       <c r="H11" s="2">
         <v>96.148514988790296</v>
       </c>
-      <c r="I11" s="4">
-        <v>1.1299999999999999</v>
+      <c r="I11" s="6">
+        <v>0.79479330984803698</v>
       </c>
       <c r="J11" s="4">
-        <v>100</v>
-      </c>
-      <c r="K11" s="4">
-        <v>1.1299999999999999</v>
+        <v>92</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0.79479330984803698</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B12" s="4">
         <v>76.08</v>
       </c>
-      <c r="C12" s="4">
-        <v>0.41</v>
+      <c r="C12" s="6">
+        <v>0.30047254544477298</v>
       </c>
       <c r="D12" s="4">
         <v>89.85</v>
       </c>
-      <c r="E12" s="4">
-        <v>0.41</v>
+      <c r="E12" s="6">
+        <v>0.30047254544477298</v>
       </c>
       <c r="F12" s="1">
         <v>90.97</v>
       </c>
-      <c r="G12" s="4">
-        <v>0.41</v>
+      <c r="G12" s="6">
+        <v>0.30047254544477298</v>
       </c>
       <c r="H12" s="2">
         <v>95.842222057607799</v>
       </c>
-      <c r="I12" s="4">
-        <v>0.41</v>
+      <c r="I12" s="6">
+        <v>0.30047254544477298</v>
       </c>
       <c r="J12" s="4">
-        <v>100</v>
-      </c>
-      <c r="K12" s="4">
-        <v>0.41</v>
+        <v>92</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0.30047254544477298</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B13" s="4">
         <v>78.290000000000006</v>
       </c>
-      <c r="C13" s="4">
-        <v>0.43</v>
+      <c r="C13" s="6">
+        <v>0.36518423585221799</v>
       </c>
       <c r="D13" s="4">
         <v>89.97</v>
       </c>
-      <c r="E13" s="4">
-        <v>0.43</v>
+      <c r="E13" s="6">
+        <v>0.36518423585221799</v>
       </c>
       <c r="F13" s="1">
         <v>90.03</v>
       </c>
-      <c r="G13" s="4">
-        <v>0.43</v>
+      <c r="G13" s="6">
+        <v>0.36518423585221799</v>
       </c>
       <c r="H13" s="2">
         <v>92.799203888301406</v>
       </c>
-      <c r="I13" s="4">
-        <v>0.43</v>
+      <c r="I13" s="6">
+        <v>0.36518423585221799</v>
       </c>
       <c r="J13" s="4">
-        <v>100</v>
-      </c>
-      <c r="K13" s="4">
-        <v>0.43</v>
+        <v>92</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0.36518423585221799</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B14" s="4">
         <v>57.46</v>
       </c>
-      <c r="C14" s="4">
-        <v>1.1000000000000001</v>
+      <c r="C14" s="6">
+        <v>0.52270993834590096</v>
       </c>
       <c r="D14" s="4">
         <v>78.81</v>
       </c>
-      <c r="E14" s="4">
-        <v>1.1000000000000001</v>
+      <c r="E14" s="6">
+        <v>0.52270993834590096</v>
       </c>
       <c r="F14" s="1">
         <v>81.150000000000006</v>
       </c>
-      <c r="G14" s="4">
-        <v>1.1000000000000001</v>
+      <c r="G14" s="6">
+        <v>0.52270993834590096</v>
       </c>
       <c r="H14" s="2">
         <v>88.334653784167202</v>
       </c>
-      <c r="I14" s="4">
-        <v>1.1000000000000001</v>
+      <c r="I14" s="6">
+        <v>0.52270993834590096</v>
       </c>
       <c r="J14" s="4">
-        <v>100</v>
-      </c>
-      <c r="K14" s="4">
-        <v>1.1000000000000001</v>
+        <v>92</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0.52270993834590096</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B15" s="4">
         <v>63.92</v>
       </c>
-      <c r="C15" s="4">
-        <v>3.05</v>
+      <c r="C15" s="6">
+        <v>0.76606466194907796</v>
       </c>
       <c r="D15" s="4">
         <v>83.18</v>
       </c>
-      <c r="E15" s="4">
-        <v>3.05</v>
+      <c r="E15" s="6">
+        <v>0.76606466194907796</v>
       </c>
       <c r="F15" s="1">
         <v>84.46</v>
       </c>
-      <c r="G15" s="4">
-        <v>3.05</v>
+      <c r="G15" s="6">
+        <v>0.76606466194907796</v>
       </c>
       <c r="H15" s="2">
         <v>91.186976647721096</v>
       </c>
-      <c r="I15" s="4">
-        <v>3.05</v>
+      <c r="I15" s="6">
+        <v>0.76606466194907796</v>
       </c>
       <c r="J15" s="4">
-        <v>100</v>
-      </c>
-      <c r="K15" s="4">
-        <v>3.05</v>
+        <v>92</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0.76606466194907796</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B16" s="4">
         <v>62.39</v>
       </c>
-      <c r="C16" s="4">
-        <v>2.0299999999999998</v>
+      <c r="C16" s="6">
+        <v>0.87819748870578296</v>
       </c>
       <c r="D16" s="4">
         <v>84.64</v>
       </c>
-      <c r="E16" s="4">
-        <v>2.0299999999999998</v>
+      <c r="E16" s="6">
+        <v>0.87819748870578296</v>
       </c>
       <c r="F16" s="1">
         <v>86.55</v>
       </c>
-      <c r="G16" s="4">
-        <v>2.0299999999999998</v>
+      <c r="G16" s="6">
+        <v>0.87819748870578296</v>
       </c>
       <c r="H16" s="2">
         <v>91.850017906641497</v>
       </c>
-      <c r="I16" s="4">
-        <v>2.0299999999999998</v>
+      <c r="I16" s="6">
+        <v>0.87819748870578296</v>
       </c>
       <c r="J16" s="4">
-        <v>100</v>
-      </c>
-      <c r="K16" s="4">
-        <v>2.0299999999999998</v>
+        <v>92</v>
+      </c>
+      <c r="K16" s="6">
+        <v>0.87819748870578296</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B17" s="4">
-        <v>72.14</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0.49</v>
-      </c>
-      <c r="D17" s="4">
-        <v>90.82</v>
-      </c>
-      <c r="E17" s="4">
-        <v>0.49</v>
-      </c>
-      <c r="F17" s="1">
-        <v>83.17</v>
-      </c>
-      <c r="G17" s="4">
-        <v>0.49</v>
-      </c>
-      <c r="H17" s="2">
-        <v>93</v>
-      </c>
-      <c r="I17" s="4">
-        <v>0.49</v>
-      </c>
-      <c r="J17" s="4">
-        <v>100</v>
-      </c>
-      <c r="K17" s="4">
-        <v>0.49</v>
+        <v>57</v>
+      </c>
+      <c r="B17" s="5">
+        <f t="shared" ref="B17:K17" si="0">AVERAGE(B2:B16)</f>
+        <v>67.951999999999998</v>
+      </c>
+      <c r="C17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.71515270692371946</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" si="0"/>
+        <v>83.852666666666678</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.71515270692371946</v>
+      </c>
+      <c r="F17" s="5">
+        <f t="shared" si="0"/>
+        <v>85.13600000000001</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.71515270692371946</v>
+      </c>
+      <c r="H17" s="5">
+        <f t="shared" si="0"/>
+        <v>90.480682037677894</v>
+      </c>
+      <c r="I17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.71515270692371946</v>
+      </c>
+      <c r="J17" s="5">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="K17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.71515270692371946</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B18" s="4">
-        <f t="shared" ref="B18:I18" si="0">AVERAGE(B2:B17)</f>
-        <v>68.213750000000005</v>
-      </c>
-      <c r="C18" s="5">
-        <f t="shared" si="0"/>
-        <v>1.8325000000000002</v>
-      </c>
-      <c r="D18" s="4">
-        <f t="shared" si="0"/>
-        <v>84.288125000000008</v>
-      </c>
-      <c r="E18" s="5">
-        <f t="shared" si="0"/>
-        <v>1.8325000000000002</v>
-      </c>
-      <c r="F18" s="4">
-        <f t="shared" si="0"/>
-        <v>85.013125000000016</v>
-      </c>
-      <c r="G18" s="5">
-        <f t="shared" si="0"/>
-        <v>1.8325000000000002</v>
-      </c>
-      <c r="H18" s="4">
-        <f t="shared" si="0"/>
-        <v>90.638139410323021</v>
-      </c>
-      <c r="I18" s="5">
-        <f t="shared" si="0"/>
-        <v>1.8325000000000002</v>
-      </c>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="C19" s="6">
+        <v>70</v>
+      </c>
+      <c r="C18" s="6">
         <f>PEARSON(C2:C16,B2:B16)</f>
-        <v>-0.44902910842052818</v>
-      </c>
-      <c r="E19" s="6">
+        <v>-0.46955505643386997</v>
+      </c>
+      <c r="E18" s="6">
         <f>PEARSON(E2:E16,D2:D16)</f>
-        <v>-0.44692693733318228</v>
-      </c>
-      <c r="G19" s="6">
+        <v>-0.36534415686336691</v>
+      </c>
+      <c r="G18" s="6">
         <f>PEARSON(G2:G16,F2:F16)</f>
-        <v>-0.43176846348184744</v>
-      </c>
-      <c r="I19" s="6">
+        <v>-0.33536124667708539</v>
+      </c>
+      <c r="I18" s="6">
         <f>PEARSON(I2:I16,H2:H16)</f>
-        <v>-0.42142210409257042</v>
-      </c>
-      <c r="K19" s="6"/>
+        <v>-0.35573460594778766</v>
+      </c>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="4">
+        <v>72.14</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.49</v>
+      </c>
+      <c r="D21" s="4">
+        <v>90.82</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.49</v>
+      </c>
+      <c r="F21" s="1">
+        <v>83.17</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0.49</v>
+      </c>
+      <c r="H21" s="2">
+        <v>93</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0.49</v>
+      </c>
+      <c r="J21" s="4">
+        <v>100</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0.49</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added Yandi's partial results on Ebates
</commit_message>
<xml_diff>
--- a/coling2016/props/Ebates-COLING-2016-results.xlsx
+++ b/coling2016/props/Ebates-COLING-2016-results.xlsx
@@ -1858,7 +1858,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2017,11 +2016,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2114122120"/>
-        <c:axId val="-2123534968"/>
+        <c:axId val="-2066184616"/>
+        <c:axId val="-2065552648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2114122120"/>
+        <c:axId val="-2066184616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2051,7 +2050,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2123534968"/>
+        <c:crossAx val="-2065552648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2059,7 +2058,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2123534968"/>
+        <c:axId val="-2065552648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2080,7 +2079,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114122120"/>
+        <c:crossAx val="-2066184616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2127,7 +2126,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2287,11 +2285,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2114335768"/>
-        <c:axId val="-2114832920"/>
+        <c:axId val="-2067973096"/>
+        <c:axId val="-2064983848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2114335768"/>
+        <c:axId val="-2067973096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2321,7 +2319,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114832920"/>
+        <c:crossAx val="-2064983848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2329,7 +2327,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114832920"/>
+        <c:axId val="-2064983848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80.0"/>
@@ -2352,7 +2350,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114335768"/>
+        <c:crossAx val="-2067973096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3044,28 +3042,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>92.0</c:v>
+                  <c:v>82.9531565493</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>92.0</c:v>
+                  <c:v>86.4627168819</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>92.0</c:v>
+                  <c:v>89.7175014385</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>92.0</c:v>
+                  <c:v>76.732054123</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>92.0</c:v>
+                  <c:v>93.0942446656</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>92.0</c:v>
@@ -3077,16 +3075,16 @@
                   <c:v>92.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>92.0</c:v>
+                  <c:v>92.4780639683</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>92.0</c:v>
+                  <c:v>87.9418777705</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>92.0</c:v>
+                  <c:v>89.9320042744</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>92.0</c:v>
+                  <c:v>89.10311585469999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3103,11 +3101,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2114971352"/>
-        <c:axId val="-2114274664"/>
+        <c:axId val="-2120347192"/>
+        <c:axId val="-2071804184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2114971352"/>
+        <c:axId val="-2120347192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3139,7 +3137,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114274664"/>
+        <c:crossAx val="-2071804184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3147,7 +3145,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114274664"/>
+        <c:axId val="-2071804184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3192,7 +3190,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114971352"/>
+        <c:crossAx val="-2120347192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
@@ -4372,7 +4370,7 @@
   <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G2"/>
+      <selection activeCell="G3" sqref="G3:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4435,7 +4433,7 @@
         <v>86.320642119120095</v>
       </c>
       <c r="G3" s="2">
-        <v>92</v>
+        <v>82.953156549300004</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4481,7 +4479,7 @@
         <v>91.024201633065303</v>
       </c>
       <c r="G5" s="2">
-        <v>92</v>
+        <v>86.462716881900008</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4504,7 +4502,7 @@
         <v>90.432399190786796</v>
       </c>
       <c r="G6" s="2">
-        <v>92</v>
+        <v>89.717501438500008</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4550,7 +4548,7 @@
         <v>77.488465174735197</v>
       </c>
       <c r="G8" s="2">
-        <v>92</v>
+        <v>76.732054122999998</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4596,7 +4594,7 @@
         <v>94.945618910563695</v>
       </c>
       <c r="G10" s="2">
-        <v>92</v>
+        <v>93.094244665600002</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -4688,7 +4686,7 @@
         <v>92.799203888301406</v>
       </c>
       <c r="G14" s="2">
-        <v>92</v>
+        <v>92.478063968299992</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4711,7 +4709,7 @@
         <v>88.334653784167202</v>
       </c>
       <c r="G15" s="2">
-        <v>92</v>
+        <v>87.9418777705</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -4734,7 +4732,7 @@
         <v>91.186976647721096</v>
       </c>
       <c r="G16" s="2">
-        <v>92</v>
+        <v>89.932004274400001</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -4757,7 +4755,7 @@
         <v>91.850017906641497</v>
       </c>
       <c r="G17" s="2">
-        <v>92</v>
+        <v>89.103115854699993</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -4802,7 +4800,7 @@
       </c>
       <c r="G19" s="2">
         <f>AVERAGE(G3:G18)</f>
-        <v>92</v>
+        <v>89.525920970387503</v>
       </c>
     </row>
     <row r="26" spans="1:11">

</xml_diff>

<commit_message>
updating paper and removing auxilliary files
</commit_message>
<xml_diff>
--- a/coling2016/props/Ebates-COLING-2016-results.xlsx
+++ b/coling2016/props/Ebates-COLING-2016-results.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="630" activeTab="1"/>
+    <workbookView xWindow="1740" yWindow="1680" windowWidth="25600" windowHeight="16060" tabRatio="630" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DatasetStats" sheetId="14" r:id="rId1"/>
     <sheet name="Predictions" sheetId="15" r:id="rId2"/>
     <sheet name="KLvsPrediction" sheetId="16" r:id="rId3"/>
+    <sheet name="Earlier" sheetId="17" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="87">
   <si>
     <t>Categories</t>
   </si>
@@ -243,6 +244,45 @@
   </si>
   <si>
     <t>CNN w/ pretraining</t>
+  </si>
+  <si>
+    <t>92 is a placeholder</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>LogReg L1 Micro F1</t>
+  </si>
+  <si>
+    <t>XGboost Micro Precision</t>
+  </si>
+  <si>
+    <t>XGboost Micro F1</t>
+  </si>
+  <si>
+    <t>Baby and Kids Clothes</t>
+  </si>
+  <si>
+    <t>Jewelry and Watches</t>
+  </si>
+  <si>
+    <t>Bags, Handbags and Accessories</t>
+  </si>
+  <si>
+    <t>Health, Beauty and Fragrance</t>
+  </si>
+  <si>
+    <t>Electronics and Computers</t>
+  </si>
+  <si>
+    <t>Sports and Fitness</t>
+  </si>
+  <si>
+    <t>Home, Patio and Furniture</t>
+  </si>
+  <si>
+    <t>LogReg L1 Micro Precision</t>
   </si>
 </sst>
 </file>
@@ -317,7 +357,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="738">
+  <cellStyleXfs count="746">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1056,8 +1096,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1068,8 +1116,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="738">
+  <cellStyles count="746">
     <cellStyle name="Comma 2" xfId="95"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1439,6 +1490,10 @@
     <cellStyle name="Followed Hyperlink" xfId="733" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="735" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="737" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="739" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="741" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="743" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="745" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1807,6 +1862,10 @@
     <cellStyle name="Hyperlink" xfId="732" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="734" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="736" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="738" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="740" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="742" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="744" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2016,11 +2075,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2066184616"/>
-        <c:axId val="-2065552648"/>
+        <c:axId val="-2054935560"/>
+        <c:axId val="-2054932376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2066184616"/>
+        <c:axId val="-2054935560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2050,7 +2109,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2065552648"/>
+        <c:crossAx val="-2054932376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2058,7 +2117,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2065552648"/>
+        <c:axId val="-2054932376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2079,7 +2138,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2066184616"/>
+        <c:crossAx val="-2054935560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2285,11 +2344,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2067973096"/>
-        <c:axId val="-2064983848"/>
+        <c:axId val="-2145232200"/>
+        <c:axId val="-2076806408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2067973096"/>
+        <c:axId val="-2145232200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2319,7 +2378,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2064983848"/>
+        <c:crossAx val="-2076806408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2327,7 +2386,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2064983848"/>
+        <c:axId val="-2076806408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80.0"/>
@@ -2350,7 +2409,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2067973096"/>
+        <c:crossAx val="-2145232200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3101,11 +3160,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2120347192"/>
-        <c:axId val="-2071804184"/>
+        <c:axId val="-2079183304"/>
+        <c:axId val="-2079077448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2120347192"/>
+        <c:axId val="-2079183304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3137,7 +3196,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071804184"/>
+        <c:crossAx val="-2079077448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3145,7 +3204,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2071804184"/>
+        <c:axId val="-2079077448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -3190,7 +3249,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2120347192"/>
+        <c:crossAx val="-2079183304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
@@ -3215,6 +3274,520 @@
         <a:p>
           <a:pPr>
             <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="120"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="20"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" cap="small"/>
+              <a:t>State-of-the-art</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" cap="small" baseline="0"/>
+              <a:t> Level 1 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" cap="small"/>
+              <a:t>Classifier MICRO Performance Comparison</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.119148100972673"/>
+          <c:y val="0.0195530726256983"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.123245708416883"/>
+          <c:y val="0.127374301675978"/>
+          <c:w val="0.416764474293654"/>
+          <c:h val="0.320491576122817"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Earlier!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LogReg L1 Micro Precision</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Earlier!$A$3:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Toys</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Home, Patio and Furniture</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Jewelry and Watches</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Bags, Handbags and Accessories</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Health, Beauty and Fragrance</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Shoes</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Electronics and Computers</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Office</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sports and Fitness</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Automotive</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Industrial</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Baby Products</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Baby and Kids Clothes</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Men's Clothing</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Women's Clothing</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Earlier!$B$3:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>76.004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>84.00200000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80.894</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81.676</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.178</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.516</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80.132</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>89.21799999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>83.57199999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>88.794</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>88.23600000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>88.19000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>89.034</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>82.41999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>83.362</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Earlier!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LogReg L1 Micro F1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="75000"/>
+                <a:alpha val="72000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Earlier!$A$3:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Toys</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Home, Patio and Furniture</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Jewelry and Watches</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Bags, Handbags and Accessories</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Health, Beauty and Fragrance</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Shoes</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Electronics and Computers</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Office</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sports and Fitness</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Automotive</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Industrial</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Baby Products</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Baby and Kids Clothes</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Men's Clothing</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Women's Clothing</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Earlier!$C$3:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>76.004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>84.00200000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80.894</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81.676</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.178</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.516</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80.132</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>89.21799999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>83.57199999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>88.794</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>88.23600000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>88.19000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>89.034</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>82.41999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>83.362</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2141082760"/>
+        <c:axId val="-2078403848"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2141082760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="165100" dist="25400" dir="2700000" sx="93000" sy="93000" algn="tl" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="13000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" vert="horz" lIns="2" anchor="ctr" anchorCtr="1">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" kern="1200" cap="none" spc="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2078403848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2078403848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100.0"/>
+          <c:min val="60.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="3175" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:alpha val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" cap="small"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" cap="small"/>
+                  <a:t>Prediction Micro Precision/F1</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.040774548402038"/>
+              <c:y val="0.101507720054546"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:effectLst>
+            <a:outerShdw blurRad="95250" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="22000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" baseline="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2141082760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5.0"/>
+        <c:minorUnit val="2.0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.54192276516906"/>
+          <c:y val="0.139110324198302"/>
+          <c:w val="0.193499884205651"/>
+          <c:h val="0.198315664452558"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" cap="small"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -3320,6 +3893,43 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4370,7 +4980,7 @@
   <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G19"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4385,13 +4995,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" t="s">
@@ -4818,6 +5428,9 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
+      <c r="G27" t="s">
+        <v>74</v>
+      </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -4964,11 +5577,11 @@
       <c r="K41" s="2"/>
     </row>
     <row r="77" spans="2:6">
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="7"/>
-      <c r="F77" s="7"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
     </row>
     <row r="79" spans="2:6">
       <c r="C79" s="2"/>
@@ -4995,9 +5608,9 @@
       <c r="F82" s="2"/>
     </row>
     <row r="84" spans="2:6">
-      <c r="B84" s="7"/>
-      <c r="C84" s="7"/>
-      <c r="D84" s="7"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
     </row>
@@ -5721,4 +6334,301 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5">
+      <c r="A2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>76.003999999999991</v>
+      </c>
+      <c r="C3">
+        <v>76.003999999999991</v>
+      </c>
+      <c r="D3">
+        <v>81.347999999999999</v>
+      </c>
+      <c r="E3">
+        <v>81.347999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4">
+        <v>84.00200000000001</v>
+      </c>
+      <c r="C4">
+        <v>84.00200000000001</v>
+      </c>
+      <c r="D4">
+        <v>88.9</v>
+      </c>
+      <c r="E4">
+        <v>88.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5">
+        <v>80.894000000000005</v>
+      </c>
+      <c r="C5">
+        <v>80.894000000000005</v>
+      </c>
+      <c r="D5">
+        <v>86.027999999999992</v>
+      </c>
+      <c r="E5">
+        <v>86.027999999999992</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6">
+        <v>81.676000000000002</v>
+      </c>
+      <c r="C6">
+        <v>81.676000000000002</v>
+      </c>
+      <c r="D6">
+        <v>85.001999999999995</v>
+      </c>
+      <c r="E6">
+        <v>85.001999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7">
+        <v>82.177999999999997</v>
+      </c>
+      <c r="C7">
+        <v>82.177999999999997</v>
+      </c>
+      <c r="D7">
+        <v>85.390000000000015</v>
+      </c>
+      <c r="E7">
+        <v>85.390000000000015</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8">
+        <v>64.516000000000005</v>
+      </c>
+      <c r="C8">
+        <v>64.516000000000005</v>
+      </c>
+      <c r="D8">
+        <v>66.608000000000004</v>
+      </c>
+      <c r="E8">
+        <v>66.608000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9">
+        <v>80.132000000000005</v>
+      </c>
+      <c r="C9">
+        <v>80.132000000000005</v>
+      </c>
+      <c r="D9">
+        <v>84.496000000000009</v>
+      </c>
+      <c r="E9">
+        <v>84.496000000000009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10">
+        <v>89.217999999999989</v>
+      </c>
+      <c r="C10">
+        <v>89.217999999999989</v>
+      </c>
+      <c r="D10">
+        <v>92.891999999999996</v>
+      </c>
+      <c r="E10">
+        <v>92.891999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11">
+        <v>83.571999999999989</v>
+      </c>
+      <c r="C11">
+        <v>83.571999999999989</v>
+      </c>
+      <c r="D11">
+        <v>87.443999999999988</v>
+      </c>
+      <c r="E11">
+        <v>87.443999999999988</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12">
+        <v>88.794000000000011</v>
+      </c>
+      <c r="C12">
+        <v>88.794000000000011</v>
+      </c>
+      <c r="D12">
+        <v>94.753999999999991</v>
+      </c>
+      <c r="E12">
+        <v>94.753999999999991</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>88.236000000000018</v>
+      </c>
+      <c r="C13">
+        <v>88.236000000000018</v>
+      </c>
+      <c r="D13">
+        <v>93.137999999999991</v>
+      </c>
+      <c r="E13">
+        <v>93.137999999999991</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14">
+        <v>88.190000000000012</v>
+      </c>
+      <c r="C14">
+        <v>88.190000000000012</v>
+      </c>
+      <c r="D14">
+        <v>89.671999999999997</v>
+      </c>
+      <c r="E14">
+        <v>89.671999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15">
+        <v>89.033999999999992</v>
+      </c>
+      <c r="C15">
+        <v>89.033999999999992</v>
+      </c>
+      <c r="D15">
+        <v>92.140000000000015</v>
+      </c>
+      <c r="E15">
+        <v>92.140000000000015</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16">
+        <v>82.419999999999987</v>
+      </c>
+      <c r="C16">
+        <v>82.419999999999987</v>
+      </c>
+      <c r="D16">
+        <v>85.464000000000013</v>
+      </c>
+      <c r="E16">
+        <v>85.464000000000013</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17">
+        <v>83.361999999999995</v>
+      </c>
+      <c r="C17">
+        <v>83.361999999999995</v>
+      </c>
+      <c r="D17">
+        <v>85.468000000000004</v>
+      </c>
+      <c r="E17">
+        <v>85.468000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>